<commit_message>
Examples checked and working
</commit_message>
<xml_diff>
--- a/example/apples.xlsx
+++ b/example/apples.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\excel_to_gorm\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{38D31206-A4AE-4E21-90F1-D8EE7E801B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77964264-2C31-4F75-9D94-95E1BCD050AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
+    <workbookView xWindow="31275" yWindow="-2460" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="colMap-apples" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Germany</t>
   </si>
   <si>
-    <t>Iraq</t>
-  </si>
-  <si>
     <t>Fred Bloggs</t>
   </si>
   <si>
@@ -123,12 +120,6 @@
   </si>
   <si>
     <t>Nash Bridges</t>
-  </si>
-  <si>
-    <t>Saaed Khalifa</t>
-  </si>
-  <si>
-    <t>Tariq Hashim</t>
   </si>
   <si>
     <t>Navel Orange</t>
@@ -146,7 +137,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -992,7 +983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1132,7 +1123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1157,7 +1148,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5">
         <v>9.8000000000000007</v>
@@ -1168,7 +1159,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B3" s="5">
         <v>8.6999999999999993</v>
@@ -1179,7 +1170,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" s="5">
         <v>10.3</v>
@@ -1190,7 +1181,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" s="5">
         <v>11.2</v>
@@ -1205,7 +1196,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1338,7 +1329,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1443,11 +1434,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G16:G17"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,10 +1490,10 @@
         <v>1390</v>
       </c>
       <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1522,10 +1513,10 @@
         <v>3445</v>
       </c>
       <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
         <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1545,10 +1536,10 @@
         <v>221458</v>
       </c>
       <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
         <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1568,33 +1559,10 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>